<commit_message>
Refactor: Implement trigger-based menu swapping and strict 6-row block structure
</commit_message>
<xml_diff>
--- a/data/kondate_K001_2026_2.xlsx
+++ b/data/kondate_K001_2026_2.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,474 +445,288 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Day</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
           <t>Menu</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Ingredients</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Energy (kcal)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46055</v>
+        <v>46054</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>ポテト
-ポテト</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
-        <v>0</v>
+          <t>Allergy Dish 1</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46056</v>
+        <v>46055</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Tue</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>さつまあげ</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>さつま揚げ</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
+          <t>Dish 2-1, Dish 2-2</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46057</v>
+        <v>46056</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ブロッコリー
-マカロニサラダ</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>ﾊﾑ</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
+          <t>Dish 3-1, Dish 3-2</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46058</v>
+        <v>46057</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Thu</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>きんぴられんこん</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="n">
-        <v>0</v>
+          <t>Dish 4-1, Dish 4-2</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>46059</v>
+        <v>46058</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>コロッケ
-あつあげとチンゲンさいのいためもの</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>厚揚げ</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
+          <t>Dish 5-1, Dish 5-2</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>46062</v>
+        <v>46059</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ミートボールのケチャップあえ
-ミートボールのケチャップあえ</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>ﾐｰﾄﾎﾞｰﾙ
-ﾐｰﾄﾎﾞｰﾙ</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
+          <t>Dish 6-1, Dish 6-2</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>46063</v>
+        <v>46060</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Tue</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>コーン
-コーン</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="n">
-        <v>0</v>
+          <t>Dish 7-1, Dish 7-2</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>46064</v>
+        <v>46061</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>けんこくきねんのひ</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="n">
-        <v>0</v>
+          <t>Dish 8-1, Dish 8-2</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>46065</v>
+        <v>46062</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Thu</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>にんじんシリシリ
-にんじんシリシリ</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>ﾂﾅ
-ﾂﾅ</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
+          <t>Dish 9-1, Dish 9-2</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>46066</v>
+        <v>46063</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>ゆでたまご
-ゆでたまご</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>卵
-卵</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
+          <t>Dish 10-1, Dish 10-2</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>46069</v>
+        <v>46064</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>ペペロンチーノふうビーフン</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>ﾍﾞｰｺﾝ</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
+          <t>Dish 11-1, Dish 11-2</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>46070</v>
+        <v>46065</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Tue</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>ぎょうざ
-ぎょうざ</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>ぎょうざ
-ぎょうざ</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
+          <t>Dish 12-1, Dish 12-2</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>46071</v>
+        <v>46066</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>スパゲティソテー
-スパニッシュエッグ</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>卵</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>0</v>
+          <t>Dish 13-1, Dish 13-2</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>46072</v>
+        <v>46067</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Thu</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>オムレツ</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>ｵﾑﾚﾂ</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>0</v>
+          <t>Dish 14-1, Dish 14-2</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>46073</v>
+        <v>46068</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>ちくわのいそべてん
-なすとマカロニのトマトあえ</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>ちくわ　青のり
-合挽肉</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>0</v>
+          <t>Dish 15-1, Dish 15-2</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>46076</v>
+        <v>46069</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>てんのうたんじょうび</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="n">
-        <v>0</v>
+          <t>Dish 16-1, Dish 16-2</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>46077</v>
+        <v>46070</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Tue</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>たまごやき
-たまごやき</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>卵焼き
-卵焼き</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>0</v>
+          <t>Dish 17-1, Dish 17-2</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>46078</v>
+        <v>46071</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>ウィンナー</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>ｳｨﾝﾅｰ</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
-        <v>0</v>
+          <t>Dish 18-1, Dish 18-2</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>46079</v>
+        <v>46072</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Thu</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>きんぴられんこん
-いもいもサラダ</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="n">
-        <v>0</v>
+          <t>Dish 19-1, Dish 19-2</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
+        <v>46073</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Dish 20-1, Dish 20-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>46074</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Dish 21-1, Dish 21-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>46075</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Dish 22-1, Dish 22-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>46076</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Dish 23-1, Dish 23-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>46077</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Dish 24-1, Dish 24-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>46078</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Dish 25-1, Dish 25-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>46079</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Dish 26-1, Dish 26-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
         <v>46080</v>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>ほうれんそうのおひたし
-ほうれんそうのおひたし</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="n">
-        <v>0</v>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Dish 27-1, Dish 27-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>46081</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Dish 28-1, Dish 28-2</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>